<commit_message>
Add file phân tích công việc tuần 1 - Đưa ra vấn đề gặp phải
</commit_message>
<xml_diff>
--- a/04. Ke Hoach/02. Ke hoach nhom/191029_KehoachNhom.xlsx
+++ b/04. Ke Hoach/02. Ke hoach nhom/191029_KehoachNhom.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -294,15 +294,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -315,6 +306,15 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -599,18 +599,18 @@
   <dimension ref="A1:T34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" style="1" customWidth="1"/>
-    <col min="2" max="4" width="9.109375" style="1"/>
-    <col min="5" max="5" width="12.109375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="10.5546875" style="1" customWidth="1"/>
-    <col min="7" max="9" width="9.109375" style="1"/>
-    <col min="10" max="10" width="12.6640625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="1" width="6.5703125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="9.140625" style="1"/>
+    <col min="5" max="5" width="12.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="1" customWidth="1"/>
+    <col min="7" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="12.7109375" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -622,38 +622,38 @@
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
-      <c r="E4" s="30"/>
-      <c r="F4" s="30" t="s">
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="33" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="30"/>
-      <c r="H4" s="30"/>
-      <c r="I4" s="30"/>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30" t="s">
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30" t="s">
+      <c r="L4" s="33"/>
+      <c r="M4" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30" t="s">
+      <c r="N4" s="33"/>
+      <c r="O4" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="P4" s="30"/>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="29">
+      <c r="A5" s="34">
         <v>1</v>
       </c>
       <c r="B5" s="16" t="s">
@@ -681,7 +681,7 @@
       <c r="T5" s="18"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="29"/>
+      <c r="A6" s="34"/>
       <c r="B6" s="20"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
@@ -705,7 +705,7 @@
       <c r="T6" s="22"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="29"/>
+      <c r="A7" s="34"/>
       <c r="B7" s="20"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
@@ -727,7 +727,7 @@
       <c r="T7" s="22"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
+      <c r="A8" s="34"/>
       <c r="B8" s="24"/>
       <c r="C8" s="25"/>
       <c r="D8" s="25"/>
@@ -749,7 +749,7 @@
       <c r="T8" s="26"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+      <c r="A9" s="35">
         <v>2</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -777,7 +777,7 @@
       <c r="T9" s="7"/>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="28"/>
+      <c r="A10" s="35"/>
       <c r="B10" s="9"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -801,7 +801,7 @@
       <c r="T10" s="11"/>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="28"/>
+      <c r="A11" s="35"/>
       <c r="B11" s="9"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -823,7 +823,7 @@
       <c r="T11" s="11"/>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="28"/>
+      <c r="A12" s="35"/>
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
@@ -845,7 +845,7 @@
       <c r="T12" s="15"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="29">
+      <c r="A13" s="34">
         <v>3</v>
       </c>
       <c r="B13" s="16" t="s">
@@ -873,7 +873,7 @@
       <c r="T13" s="18"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
+      <c r="A14" s="34"/>
       <c r="B14" s="20"/>
       <c r="C14" s="21"/>
       <c r="D14" s="21"/>
@@ -897,7 +897,7 @@
       <c r="T14" s="22"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
+      <c r="A15" s="34"/>
       <c r="B15" s="20"/>
       <c r="C15" s="21"/>
       <c r="D15" s="21"/>
@@ -921,7 +921,7 @@
       <c r="T15" s="22"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
+      <c r="A16" s="34"/>
       <c r="B16" s="24"/>
       <c r="C16" s="25"/>
       <c r="D16" s="25"/>
@@ -945,7 +945,7 @@
       <c r="T16" s="26"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A17" s="28">
+      <c r="A17" s="35">
         <v>4</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -961,10 +961,10 @@
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
       <c r="J17" s="7"/>
-      <c r="K17" s="32" t="s">
+      <c r="K17" s="29" t="s">
         <v>23</v>
       </c>
-      <c r="L17" s="33"/>
+      <c r="L17" s="30"/>
       <c r="M17" s="8" t="s">
         <v>24</v>
       </c>
@@ -977,7 +977,7 @@
       <c r="T17" s="7"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A18" s="28"/>
+      <c r="A18" s="35"/>
       <c r="B18" s="9"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
@@ -989,10 +989,10 @@
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="11"/>
-      <c r="K18" s="35" t="s">
+      <c r="K18" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="L18" s="34"/>
+      <c r="L18" s="31"/>
       <c r="M18" s="9"/>
       <c r="N18" s="11"/>
       <c r="O18" s="10"/>
@@ -1003,7 +1003,7 @@
       <c r="T18" s="11"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="28"/>
+      <c r="A19" s="35"/>
       <c r="B19" s="9"/>
       <c r="C19" s="10"/>
       <c r="D19" s="10"/>
@@ -1015,10 +1015,10 @@
       <c r="H19" s="10"/>
       <c r="I19" s="10"/>
       <c r="J19" s="11"/>
-      <c r="K19" s="35" t="s">
+      <c r="K19" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="L19" s="34"/>
+      <c r="L19" s="31"/>
       <c r="M19" s="9"/>
       <c r="N19" s="11"/>
       <c r="O19" s="10"/>
@@ -1029,12 +1029,12 @@
       <c r="T19" s="11"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A20" s="28"/>
+      <c r="A20" s="35"/>
       <c r="B20" s="13"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="14"/>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="28" t="s">
         <v>22</v>
       </c>
       <c r="G20" s="14"/>
@@ -1053,7 +1053,7 @@
       <c r="T20" s="15"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A21" s="29">
+      <c r="A21" s="34">
         <v>5</v>
       </c>
       <c r="B21" s="16" t="s">
@@ -1079,7 +1079,7 @@
       <c r="T21" s="18"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
+      <c r="A22" s="34"/>
       <c r="B22" s="20"/>
       <c r="C22" s="21"/>
       <c r="D22" s="21"/>
@@ -1101,7 +1101,7 @@
       <c r="T22" s="22"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
+      <c r="A23" s="34"/>
       <c r="B23" s="20"/>
       <c r="C23" s="21"/>
       <c r="D23" s="21"/>
@@ -1123,7 +1123,7 @@
       <c r="T23" s="22"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
+      <c r="A24" s="34"/>
       <c r="B24" s="24"/>
       <c r="C24" s="25"/>
       <c r="D24" s="25"/>
@@ -1176,16 +1176,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A9:A12"/>
+    <mergeCell ref="A13:A16"/>
+    <mergeCell ref="A17:A20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="B4:E4"/>
     <mergeCell ref="F4:J4"/>
     <mergeCell ref="K4:L4"/>
     <mergeCell ref="M4:N4"/>
     <mergeCell ref="O4:T4"/>
     <mergeCell ref="A5:A8"/>
-    <mergeCell ref="A9:A12"/>
-    <mergeCell ref="A13:A16"/>
-    <mergeCell ref="A17:A20"/>
-    <mergeCell ref="A21:A24"/>
-    <mergeCell ref="B4:E4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>